<commit_message>
add deleter.py and converter.py
</commit_message>
<xml_diff>
--- a/videos_history.xlsx
+++ b/videos_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,84 +555,217 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>lFlWULCpmak</t>
+          <t>dakZ-UrjA0c</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>dakZ-UrjA0c</t>
+          <t>CCZgyD4ZRYg</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CCZgyD4ZRYg</t>
+          <t>a-wDcMZfAWw</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>a-wDcMZfAWw</t>
+          <t>vyi5OGwUEkg</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>vyi5OGwUEkg</t>
+          <t>rnNRRCBlwwo</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>rnNRRCBlwwo</t>
+          <t>M5SnEhEYiRg</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>M5SnEhEYiRg</t>
+          <t>nKMa6Xgw--4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>nKMa6Xgw--4</t>
+          <t>I52eefwAKDE</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>I52eefwAKDE</t>
+          <t>QmrU94FzTSI</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>QmrU94FzTSI</t>
+          <t>jVKxHKVT5Dg</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>jVKxHKVT5Dg</t>
+          <t>w46bWxS9IjY</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>w46bWxS9IjY</t>
+          <t>dhZUsNJ-LQU</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>j2r2nDhTzO4</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>oadhHk2xs6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>UPOVM_oYxHc</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>y_KCK-pHzqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>eUKhgjTtxyM</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>OzWrVeC-GGw</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>IoCcF0UrQOQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>G5weJd_FwAo</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>QCUwbIQIP8E</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>0MIXDyQAjAE</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>jWeFH9QyLRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>kujwJhXRGSs</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>VYSc1h8qkgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>z-DySQ5PAAc</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>mPcLc9qgBS8</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2cTXeSVrSD0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>iOsE0eANCmA</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>gCWj8Nz5DUg</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>6WGB6lK6pAc</t>
         </is>
       </c>
     </row>

</xml_diff>